<commit_message>
Fixes #4 with inconsistancy of resistor links in electrical parts list. Also removed un maintained parts lists in the master parts list
</commit_message>
<xml_diff>
--- a/Electrical/Electrical Parts List.xlsx
+++ b/Electrical/Electrical Parts List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\osr\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\JPL Open Source Rover\open-source-rover\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,15 +164,9 @@
     <t>E22</t>
   </si>
   <si>
-    <t>CF14JT200KCT-ND</t>
-  </si>
-  <si>
     <t>Resistors 22K</t>
   </si>
   <si>
-    <t>301KXBK-ND</t>
-  </si>
-  <si>
     <t>LED Array</t>
   </si>
   <si>
@@ -191,12 +185,6 @@
     <t>http://www.batteryspace.com/li-ion-battery-14-8v-5-2ah-77wh-8a-rate-for-diving-light---un-38-3-passed.aspx</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/vishay-bc-components/MRS25000C2102FRP00/PPC21.0KZCT-ND/594966</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF18JT20K0/CF18JT20K0CT-ND/2022773</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/420</t>
   </si>
   <si>
@@ -420,6 +408,18 @@
   </si>
   <si>
     <t>https://www.amazon.com/GenBasic-Female-Solderless-Breadboard-Prototyping/dp/B01L5ULRUA/ref=sr_1_4?s=electronics&amp;ie=UTF8&amp;qid=1517958053&amp;sr=1-4&amp;keywords=female+to+female+jumper+wire</t>
+  </si>
+  <si>
+    <t>CF14JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT10K0/CF14JT10K0CT-ND/1830374</t>
+  </si>
+  <si>
+    <t>CF14JT22K0CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT22K0/CF14JT22K0CT-ND/1830383</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,14 +472,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -582,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -668,10 +660,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -713,25 +702,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1013,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1030,7 +1028,7 @@
     <col min="11" max="11" width="52.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -1170,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1205,7 +1203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1240,7 +1238,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>27</v>
       </c>
@@ -1310,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1342,10 +1340,10 @@
         <v>86.95</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
@@ -1380,7 +1378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
@@ -1399,25 +1397,27 @@
       <c r="F11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="22">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="J11" s="22">
+        <f>B11/D11*I11</f>
+        <v>0.72</v>
+      </c>
+      <c r="K11" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="M11" s="54"/>
+    </row>
+    <row r="12" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="22">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="J11" s="22">
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="B12" s="8">
         <v>25</v>
@@ -1434,25 +1434,27 @@
       <c r="F12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="28" t="s">
-        <v>48</v>
+      <c r="G12" s="52" t="s">
+        <v>130</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="22">
-        <v>3.5999999999999997E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="J12" s="22">
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <f>B12/D12*I12</f>
+        <v>0.72</v>
+      </c>
+      <c r="K12" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="M12" s="54"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="8">
         <v>1</v>
@@ -1467,7 +1469,7 @@
         <v>44</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>21</v>
@@ -1482,12 +1484,12 @@
         <v>24.95</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="17">
         <v>1</v>
@@ -1502,10 +1504,10 @@
         <v>44</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>11</v>
@@ -1517,12 +1519,12 @@
         <v>4.49</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="8">
         <v>5</v>
@@ -1534,10 +1536,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>21</v>
@@ -1552,27 +1554,27 @@
         <v>349.75</v>
       </c>
       <c r="K15" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
@@ -1587,12 +1589,12 @@
         <v>14.95</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B17" s="8">
         <v>6</v>
@@ -1604,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>21</v>
@@ -1622,12 +1624,12 @@
         <v>209.70000000000002</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B18" s="8">
         <v>4</v>
@@ -1639,10 +1641,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>21</v>
@@ -1657,12 +1659,12 @@
         <v>79.8</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" s="8">
         <v>4</v>
@@ -1674,13 +1676,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>11</v>
@@ -1692,12 +1694,12 @@
         <v>27.2</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B20" s="8">
         <v>4</v>
@@ -1709,30 +1711,30 @@
         <v>1</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="35">
         <v>55</v>
       </c>
       <c r="J20" s="22">
         <v>220</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
@@ -1750,7 +1752,7 @@
         <v>21</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>11</v>
@@ -1762,12 +1764,12 @@
         <v>6.32</v>
       </c>
       <c r="K21" s="27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B22" s="17">
         <v>1</v>
@@ -1785,7 +1787,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>11</v>
@@ -1797,12 +1799,12 @@
         <v>6.14</v>
       </c>
       <c r="K22" s="27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" s="17">
         <v>1</v>
@@ -1820,7 +1822,7 @@
         <v>21</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>11</v>
@@ -1832,12 +1834,12 @@
         <v>4.95</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B24" s="17">
         <v>1</v>
@@ -1855,7 +1857,7 @@
         <v>21</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>11</v>
@@ -1867,12 +1869,12 @@
         <v>4.95</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B25" s="17">
         <v>1</v>
@@ -1890,7 +1892,7 @@
         <v>21</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>11</v>
@@ -1902,12 +1904,12 @@
         <v>4.95</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B26" s="17">
         <v>1</v>
@@ -1925,7 +1927,7 @@
         <v>21</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>11</v>
@@ -1937,12 +1939,12 @@
         <v>4.95</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="31" t="s">
-        <v>89</v>
+      <c r="A27" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="B27" s="17">
         <v>10</v>
@@ -1957,8 +1959,8 @@
         <v>44</v>
       </c>
       <c r="F27" s="17"/>
-      <c r="G27" s="32" t="s">
-        <v>90</v>
+      <c r="G27" s="31" t="s">
+        <v>86</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>11</v>
@@ -1969,211 +1971,211 @@
       <c r="J27" s="22">
         <v>3.67</v>
       </c>
-      <c r="K27" s="37" t="s">
+      <c r="K27" s="36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="33">
+        <v>10</v>
+      </c>
+      <c r="C28" s="33">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>1</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="J28" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="K28" s="38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="33">
+        <v>1</v>
+      </c>
+      <c r="C29" s="33">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16">
+        <v>1</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="33"/>
+      <c r="G29" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="37">
+        <v>7.99</v>
+      </c>
+      <c r="J29" s="37">
+        <v>7.99</v>
+      </c>
+      <c r="K29" s="46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="39" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="34">
-        <v>10</v>
-      </c>
-      <c r="C28" s="34">
-        <v>1</v>
-      </c>
-      <c r="D28" s="16">
-        <v>1</v>
-      </c>
-      <c r="E28" s="34" t="s">
+      <c r="B30" s="33">
+        <v>1</v>
+      </c>
+      <c r="C30" s="33">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16">
+        <v>1</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="38">
-        <v>0.04</v>
-      </c>
-      <c r="J28" s="38">
-        <v>0.4</v>
-      </c>
-      <c r="K28" s="39" t="s">
+      <c r="F30" s="33"/>
+      <c r="G30" s="40" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="40" t="s">
+      <c r="H30" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="J30" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="K30" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="34">
-        <v>1</v>
-      </c>
-      <c r="C29" s="34">
-        <v>1</v>
-      </c>
-      <c r="D29" s="16">
-        <v>1</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="41" t="s">
+      <c r="B31" s="33">
+        <v>1</v>
+      </c>
+      <c r="C31" s="33">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16">
+        <v>1</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="33"/>
+      <c r="G31" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="38">
-        <v>7.99</v>
-      </c>
-      <c r="J29" s="38">
-        <v>7.99</v>
-      </c>
-      <c r="K29" s="47" t="s">
+      <c r="H31" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="37">
+        <v>12.56</v>
+      </c>
+      <c r="J31" s="37">
+        <v>12.56</v>
+      </c>
+      <c r="K31" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="33">
+        <v>1</v>
+      </c>
+      <c r="C32" s="33">
+        <v>1</v>
+      </c>
+      <c r="D32" s="16">
+        <v>1</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="J32" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="K32" s="46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="33"/>
+      <c r="G33" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="J33" s="37">
+        <v>15.59</v>
+      </c>
+      <c r="K33" s="46" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="34">
-        <v>1</v>
-      </c>
-      <c r="C30" s="34">
-        <v>1</v>
-      </c>
-      <c r="D30" s="16">
-        <v>1</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="J30" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="K30" s="47" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="34">
-        <v>1</v>
-      </c>
-      <c r="C31" s="34">
-        <v>1</v>
-      </c>
-      <c r="D31" s="16">
-        <v>1</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="38">
-        <v>12.56</v>
-      </c>
-      <c r="J31" s="38">
-        <v>12.56</v>
-      </c>
-      <c r="K31" s="48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="34">
-        <v>1</v>
-      </c>
-      <c r="C32" s="34">
-        <v>1</v>
-      </c>
-      <c r="D32" s="16">
-        <v>1</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="J32" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="K32" s="47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" s="34">
-        <v>1</v>
-      </c>
-      <c r="C33" s="34">
-        <v>1</v>
-      </c>
-      <c r="D33" s="16">
-        <v>1</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="J33" s="38">
-        <v>15.59</v>
-      </c>
-      <c r="K33" s="47" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" s="12">
         <v>5</v>
@@ -2189,7 +2191,7 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>11</v>
@@ -2201,174 +2203,174 @@
         <v>19.75</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="42">
+        <v>10</v>
+      </c>
+      <c r="C35" s="42">
+        <v>5</v>
+      </c>
+      <c r="D35" s="42">
+        <v>1</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="48">
+        <v>0.59</v>
+      </c>
+      <c r="J35" s="48">
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="K35" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="42">
+        <v>20</v>
+      </c>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42">
+        <v>1</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="48">
+        <v>0.35</v>
+      </c>
+      <c r="J36" s="48">
+        <v>7</v>
+      </c>
+      <c r="K36" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="43">
-        <v>10</v>
-      </c>
-      <c r="C35" s="43">
-        <v>5</v>
-      </c>
-      <c r="D35" s="43">
-        <v>1</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="13" t="s">
+      <c r="B37" s="42">
+        <v>1</v>
+      </c>
+      <c r="C37" s="42">
+        <v>1</v>
+      </c>
+      <c r="D37" s="42">
+        <v>1</v>
+      </c>
+      <c r="E37" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="H35" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="49">
-        <v>0.59</v>
-      </c>
-      <c r="J35" s="49">
-        <v>5.8999999999999995</v>
-      </c>
-      <c r="K35" s="50" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A36" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="43">
-        <v>20</v>
-      </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43">
-        <v>1</v>
-      </c>
-      <c r="E36" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="49">
-        <v>0.35</v>
-      </c>
-      <c r="J36" s="49">
-        <v>7</v>
-      </c>
-      <c r="K36" s="43" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A37" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="43">
-        <v>1</v>
-      </c>
-      <c r="C37" s="43">
-        <v>1</v>
-      </c>
-      <c r="D37" s="43">
-        <v>1</v>
-      </c>
-      <c r="E37" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="43" t="s">
-        <v>52</v>
+      <c r="F37" s="42" t="s">
+        <v>50</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="49">
+      <c r="H37" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="48">
         <v>20.2</v>
       </c>
-      <c r="J37" s="49">
+      <c r="J37" s="48">
         <v>20.2</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A38" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="43">
-        <v>1</v>
-      </c>
-      <c r="C38" s="43">
-        <v>1</v>
-      </c>
-      <c r="D38" s="43">
-        <v>1</v>
-      </c>
-      <c r="E38" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>120</v>
+      <c r="A38" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="42">
+        <v>1</v>
+      </c>
+      <c r="C38" s="42">
+        <v>1</v>
+      </c>
+      <c r="D38" s="42">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>116</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="49">
+      <c r="H38" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="48">
         <v>19.649999999999999</v>
       </c>
-      <c r="J38" s="49">
+      <c r="J38" s="48">
         <v>19.649999999999999</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A39" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" s="45">
+      <c r="A39" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="44">
         <v>5</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="44">
         <v>5</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="42">
         <v>1</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="46"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="45"/>
       <c r="H39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I39" s="51">
+      <c r="I39" s="50">
         <v>5.99</v>
       </c>
-      <c r="J39" s="49">
+      <c r="J39" s="48">
         <v>29.950000000000003</v>
       </c>
-      <c r="K39" s="52" t="s">
-        <v>131</v>
+      <c r="K39" s="51" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2400,6 +2402,8 @@
     <hyperlink ref="K37" r:id="rId25"/>
     <hyperlink ref="K38" r:id="rId26"/>
     <hyperlink ref="K39" r:id="rId27"/>
+    <hyperlink ref="K11" r:id="rId28"/>
+    <hyperlink ref="K12" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated parts list to include correct links to 30AWG wire.  Closes #66 and resolves #61.
</commit_message>
<xml_diff>
--- a/Electrical/Electrical Parts List.xlsx
+++ b/Electrical/Electrical Parts List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\JPL Open Source Rover\open-source-rover\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cox/Documents/open source rover/osr/Electrical/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E93500-F7BF-FE4E-9473-AED61110BC42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285"/>
+    <workbookView xWindow="56840" yWindow="4940" windowWidth="34140" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,12 +294,6 @@
     <t>CF14JT4K70CT-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2003A.11.01/C2003B-50-ND/5226402</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2015A.11.03/C2015R-50-ND/5226390</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/3169/1528-1737-ND/6193589</t>
   </si>
   <si>
@@ -420,12 +415,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT22K0/CF14JT22K0CT-ND/1830383</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/3164/1528-1732-ND/6193584</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/3164/1528-1732-ND/6193585</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -574,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -729,6 +730,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1010,25 +1014,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.33203125" customWidth="1"/>
-    <col min="2" max="6" width="14.73046875" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" customWidth="1"/>
+    <col min="2" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.73046875" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" customWidth="1"/>
-    <col min="11" max="11" width="52.19921875" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="11" max="11" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1098,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1203,7 +1207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1273,7 +1277,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>27</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
@@ -1378,7 +1382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
@@ -1398,7 +1402,7 @@
         <v>45</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>11</v>
@@ -1411,11 +1415,11 @@
         <v>0.72</v>
       </c>
       <c r="K11" s="53" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M11" s="54"/>
     </row>
-    <row r="12" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
@@ -1435,7 +1439,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>11</v>
@@ -1448,11 +1452,11 @@
         <v>0.72</v>
       </c>
       <c r="K12" s="56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M12" s="54"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
@@ -1487,7 +1491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -1522,7 +1526,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>55</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>58</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -1627,7 +1631,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>62</v>
       </c>
@@ -1662,7 +1666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>66</v>
       </c>
@@ -1697,7 +1701,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>70</v>
       </c>
@@ -1732,7 +1736,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
@@ -1758,16 +1762,16 @@
         <v>11</v>
       </c>
       <c r="I21" s="22">
-        <v>6.32</v>
+        <v>4.95</v>
       </c>
       <c r="J21" s="22">
-        <v>6.32</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+        <v>4.95</v>
+      </c>
+      <c r="K21" s="57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
@@ -1793,16 +1797,16 @@
         <v>11</v>
       </c>
       <c r="I22" s="22">
-        <v>6.14</v>
+        <v>4.95</v>
       </c>
       <c r="J22" s="22">
-        <v>6.14</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+        <v>4.95</v>
+      </c>
+      <c r="K22" s="57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>77</v>
       </c>
@@ -1834,10 +1838,10 @@
         <v>4.95</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>79</v>
       </c>
@@ -1869,10 +1873,10 @@
         <v>4.95</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>81</v>
       </c>
@@ -1904,10 +1908,10 @@
         <v>4.95</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>83</v>
       </c>
@@ -1939,10 +1943,10 @@
         <v>4.95</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>85</v>
       </c>
@@ -1972,10 +1976,10 @@
         <v>3.67</v>
       </c>
       <c r="K27" s="36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>87</v>
       </c>
@@ -2005,12 +2009,12 @@
         <v>0.4</v>
       </c>
       <c r="K28" s="38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B29" s="33">
         <v>1</v>
@@ -2026,7 +2030,7 @@
       </c>
       <c r="F29" s="33"/>
       <c r="G29" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H29" s="33" t="s">
         <v>11</v>
@@ -2038,12 +2042,12 @@
         <v>7.99</v>
       </c>
       <c r="K29" s="46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="33">
         <v>1</v>
@@ -2059,7 +2063,7 @@
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H30" s="33" t="s">
         <v>11</v>
@@ -2071,12 +2075,12 @@
         <v>15.59</v>
       </c>
       <c r="K30" s="46" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="33">
         <v>1</v>
@@ -2092,7 +2096,7 @@
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H31" s="33" t="s">
         <v>11</v>
@@ -2104,12 +2108,12 @@
         <v>12.56</v>
       </c>
       <c r="K31" s="47" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B32" s="33">
         <v>1</v>
@@ -2125,7 +2129,7 @@
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H32" s="33" t="s">
         <v>11</v>
@@ -2137,12 +2141,12 @@
         <v>15.59</v>
       </c>
       <c r="K32" s="46" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B33" s="33">
         <v>1</v>
@@ -2158,7 +2162,7 @@
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H33" s="33" t="s">
         <v>11</v>
@@ -2170,12 +2174,12 @@
         <v>15.59</v>
       </c>
       <c r="K33" s="46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="12">
         <v>5</v>
@@ -2191,7 +2195,7 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>11</v>
@@ -2203,12 +2207,12 @@
         <v>19.75</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B35" s="42">
         <v>10</v>
@@ -2224,7 +2228,7 @@
       </c>
       <c r="F35" s="42"/>
       <c r="G35" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H35" s="42" t="s">
         <v>11</v>
@@ -2236,12 +2240,12 @@
         <v>5.8999999999999995</v>
       </c>
       <c r="K35" s="49" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B36" s="42">
         <v>20</v>
@@ -2257,7 +2261,7 @@
         <v>21</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H36" s="42" t="s">
         <v>11</v>
@@ -2269,12 +2273,12 @@
         <v>7</v>
       </c>
       <c r="K36" s="42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B37" s="42">
         <v>1</v>
@@ -2286,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37" s="42" t="s">
         <v>50</v>
@@ -2304,12 +2308,12 @@
         <v>20.2</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B38" s="42">
         <v>1</v>
@@ -2321,10 +2325,10 @@
         <v>1</v>
       </c>
       <c r="E38" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="42" t="s">
         <v>114</v>
-      </c>
-      <c r="F38" s="42" t="s">
-        <v>116</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>21</v>
@@ -2339,12 +2343,12 @@
         <v>19.649999999999999</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B39" s="44">
         <v>5</v>
@@ -2370,40 +2374,41 @@
         <v>29.950000000000003</v>
       </c>
       <c r="K39" s="51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="K15" r:id="rId10"/>
-    <hyperlink ref="K16" r:id="rId11"/>
-    <hyperlink ref="K17" r:id="rId12"/>
-    <hyperlink ref="K18" r:id="rId13"/>
-    <hyperlink ref="K19" r:id="rId14"/>
-    <hyperlink ref="K20" r:id="rId15"/>
-    <hyperlink ref="K21" r:id="rId16"/>
-    <hyperlink ref="K27" r:id="rId17"/>
-    <hyperlink ref="K28" r:id="rId18"/>
-    <hyperlink ref="K29" r:id="rId19"/>
-    <hyperlink ref="K30" r:id="rId20"/>
-    <hyperlink ref="K31" r:id="rId21"/>
-    <hyperlink ref="K32" r:id="rId22"/>
-    <hyperlink ref="K33" r:id="rId23"/>
-    <hyperlink ref="K35" r:id="rId24"/>
-    <hyperlink ref="K37" r:id="rId25"/>
-    <hyperlink ref="K38" r:id="rId26"/>
-    <hyperlink ref="K39" r:id="rId27"/>
-    <hyperlink ref="K11" r:id="rId28"/>
-    <hyperlink ref="K12" r:id="rId29"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="K15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="K16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="K17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="K20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="K27" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="K28" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="K29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="K30" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="K31" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="K32" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="K33" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="K35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="K37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K38" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="K39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="K11" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="K12" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K22" r:id="rId29" xr:uid="{84B4FFE7-8258-5146-98A8-2F9119C866B9}"/>
+    <hyperlink ref="K21" r:id="rId30" xr:uid="{B92B29ED-42E6-4A4C-B16B-F3962BA7C930}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>